<commit_message>
1.  Changed run length back to inf for INTEGRATION_TEST_01.mdl 1.  Changed sequence times to 1 second intervals for testing
</commit_message>
<xml_diff>
--- a/DistributionSystems/SimulinkOpal/Device_Integration_Test_01/TestProcedure_detailed.xlsx
+++ b/DistributionSystems/SimulinkOpal/Device_Integration_Test_01/TestProcedure_detailed.xlsx
@@ -1027,7 +1027,7 @@
   <dimension ref="A1:X52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1777,7 +1777,7 @@
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
-        <v>2.7777777777777776E-2</v>
+        <v>9.2592592592592588E-5</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>40</v>
@@ -1849,7 +1849,7 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>3.125E-2</v>
+        <v>1.0416666666666667E-4</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>26</v>
@@ -1919,7 +1919,7 @@
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
-        <v>3.4722222222222224E-2</v>
+        <v>1.1574074074074073E-4</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>39</v>
@@ -1991,7 +1991,7 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
-        <v>3.8194444444444441E-2</v>
+        <v>1.273148148148148E-4</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>41</v>
@@ -2061,7 +2061,7 @@
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
-        <v>4.1666666666666664E-2</v>
+        <v>1.3888888888888889E-4</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>43</v>
@@ -2133,7 +2133,7 @@
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
-        <v>4.5138888888888888E-2</v>
+        <v>1.5046296296296297E-4</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>42</v>
@@ -2203,7 +2203,7 @@
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>4.8611111111111112E-2</v>
+        <v>1.6203703703703703E-4</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>45</v>
@@ -2273,7 +2273,7 @@
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
-        <v>5.2083333333333336E-2</v>
+        <v>1.7361111111111112E-4</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>46</v>
@@ -2345,7 +2345,7 @@
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
-        <v>5.5555555555555552E-2</v>
+        <v>1.8518518518518518E-4</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>47</v>
@@ -2415,7 +2415,7 @@
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
-        <v>5.9027777777777783E-2</v>
+        <v>1.9675925925925926E-4</v>
       </c>
       <c r="B21" s="12" t="s">
         <v>56</v>
@@ -2485,7 +2485,7 @@
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
-        <v>6.25E-2</v>
+        <v>2.0833333333333335E-4</v>
       </c>
       <c r="B22" s="12" t="s">
         <v>31</v>
@@ -2557,7 +2557,7 @@
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>6.5972222222222224E-2</v>
+        <v>2.199074074074074E-4</v>
       </c>
       <c r="B23" s="12" t="s">
         <v>44</v>
@@ -2627,7 +2627,7 @@
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
-        <v>6.9444444444444434E-2</v>
+        <v>2.3148148148148146E-4</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>176</v>
@@ -2699,7 +2699,7 @@
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>7.2916666666666671E-2</v>
+        <v>2.4305555555555552E-4</v>
       </c>
       <c r="B25" s="12" t="s">
         <v>48</v>
@@ -2769,7 +2769,7 @@
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
-        <v>7.6388888888888895E-2</v>
+        <v>2.5462962962962961E-4</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>63</v>
@@ -2841,7 +2841,7 @@
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>7.9861111111111105E-2</v>
+        <v>2.6620370370370372E-4</v>
       </c>
       <c r="B27" s="12" t="s">
         <v>50</v>
@@ -2911,7 +2911,7 @@
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="11">
-        <v>8.3333333333333329E-2</v>
+        <v>2.7777777777777778E-4</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>49</v>
@@ -2983,7 +2983,7 @@
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>8.6805555555555566E-2</v>
+        <v>2.8935185185185189E-4</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>52</v>
@@ -3053,7 +3053,7 @@
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
-        <v>9.0277777777777776E-2</v>
+        <v>3.0092592592592595E-4</v>
       </c>
       <c r="B30" s="12" t="s">
         <v>53</v>
@@ -3123,7 +3123,7 @@
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>9.375E-2</v>
+        <v>3.1250000000000001E-4</v>
       </c>
       <c r="B31" s="12" t="s">
         <v>51</v>
@@ -3193,7 +3193,7 @@
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="11">
-        <v>9.7222222222222224E-2</v>
+        <v>3.2407407407407406E-4</v>
       </c>
       <c r="B32" s="12" t="s">
         <v>57</v>
@@ -3263,7 +3263,7 @@
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
-        <v>0.10069444444444443</v>
+        <v>3.3564814814814812E-4</v>
       </c>
       <c r="B33" s="12" t="s">
         <v>44</v>
@@ -3333,7 +3333,7 @@
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" s="11">
-        <v>0.10416666666666667</v>
+        <v>3.4722222222222224E-4</v>
       </c>
       <c r="B34" s="12" t="s">
         <v>54</v>
@@ -3403,7 +3403,7 @@
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" s="11">
-        <v>0.1076388888888889</v>
+        <v>3.5879629629629635E-4</v>
       </c>
       <c r="B35" s="12" t="s">
         <v>52</v>
@@ -3473,7 +3473,7 @@
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>0.1111111111111111</v>
+        <v>3.7037037037037035E-4</v>
       </c>
       <c r="B36" s="12" t="s">
         <v>52</v>
@@ -3543,7 +3543,7 @@
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" s="11">
-        <v>0.11458333333333333</v>
+        <v>3.8194444444444446E-4</v>
       </c>
       <c r="B37" s="12" t="s">
         <v>55</v>
@@ -3613,7 +3613,7 @@
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" s="11">
-        <v>0.11805555555555557</v>
+        <v>3.9351851851851852E-4</v>
       </c>
       <c r="B38" s="12" t="s">
         <v>44</v>
@@ -3683,7 +3683,7 @@
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" s="11">
-        <v>0.12152777777777778</v>
+        <v>4.0509259259259258E-4</v>
       </c>
       <c r="B39" s="12" t="s">
         <v>39</v>
@@ -3753,7 +3753,7 @@
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" s="11">
-        <v>0.125</v>
+        <v>4.1666666666666669E-4</v>
       </c>
       <c r="B40" s="12" t="s">
         <v>66</v>
@@ -3823,7 +3823,7 @@
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>0.12847222222222224</v>
+        <v>4.2824074074074075E-4</v>
       </c>
       <c r="B41" s="12" t="s">
         <v>39</v>
@@ -3893,7 +3893,7 @@
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" s="11">
-        <v>0.13194444444444445</v>
+        <v>4.3981481481481481E-4</v>
       </c>
       <c r="B42" s="12" t="s">
         <v>44</v>
@@ -3963,7 +3963,7 @@
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>0.13541666666666666</v>
+        <v>4.5138888888888892E-4</v>
       </c>
       <c r="B43" s="12" t="s">
         <v>56</v>
@@ -4033,7 +4033,7 @@
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" s="11">
-        <v>0.1388888888888889</v>
+        <v>4.6296296296296293E-4</v>
       </c>
       <c r="B44" s="12" t="s">
         <v>58</v>
@@ -4103,7 +4103,7 @@
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" s="11">
-        <v>0.1423611111111111</v>
+        <v>4.7453703703703704E-4</v>
       </c>
       <c r="B45" s="12" t="s">
         <v>59</v>
@@ -4173,7 +4173,7 @@
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46" s="11">
-        <v>0.14583333333333334</v>
+        <v>4.8611111111111104E-4</v>
       </c>
       <c r="B46" s="12" t="s">
         <v>44</v>
@@ -4243,7 +4243,7 @@
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" s="11">
-        <v>0.14930555555555555</v>
+        <v>4.9768518518518521E-4</v>
       </c>
       <c r="B47" s="12" t="s">
         <v>60</v>
@@ -4313,7 +4313,7 @@
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>0.15277777777777776</v>
+        <v>5.0925925925925921E-4</v>
       </c>
       <c r="B48" s="12" t="s">
         <v>61</v>
@@ -4383,7 +4383,7 @@
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" s="11">
-        <v>0.15625</v>
+        <v>5.2083333333333333E-4</v>
       </c>
       <c r="B49" s="12" t="s">
         <v>36</v>
@@ -4453,7 +4453,7 @@
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>0.15972222222222224</v>
+        <v>5.3240740740740744E-4</v>
       </c>
       <c r="B50" s="12" t="s">
         <v>36</v>
@@ -4523,7 +4523,7 @@
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51" s="11">
-        <v>0.16319444444444445</v>
+        <v>5.4398148148148144E-4</v>
       </c>
       <c r="B51" s="12" t="s">
         <v>36</v>
@@ -4593,7 +4593,7 @@
     </row>
     <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52" s="11">
-        <v>0.16666666666666666</v>
+        <v>5.5555555555555556E-4</v>
       </c>
       <c r="B52" s="12" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
Added DMS to INTEGRATION_TEST_01.mdl but needs testing Made DMS intervals shorter
</commit_message>
<xml_diff>
--- a/DistributionSystems/SimulinkOpal/Device_Integration_Test_01/TestProcedure_detailed.xlsx
+++ b/DistributionSystems/SimulinkOpal/Device_Integration_Test_01/TestProcedure_detailed.xlsx
@@ -1026,8 +1026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1279,7 +1279,7 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
-        <v>3.472222222222222E-3</v>
+        <v>6.9444444444444447E-4</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>15</v>
@@ -1351,7 +1351,7 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
-        <v>6.9444444444444441E-3</v>
+        <v>1.3888888888888889E-3</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>44</v>
@@ -1421,7 +1421,7 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
-        <v>1.0416666666666666E-2</v>
+        <v>2.0833333333333333E-3</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>18</v>
@@ -1493,7 +1493,7 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
-        <v>1.3888888888888888E-2</v>
+        <v>2.7777777777777779E-3</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>44</v>
@@ -1565,7 +1565,7 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>1.7361111111111112E-2</v>
+        <v>3.472222222222222E-3</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>20</v>
@@ -1635,7 +1635,7 @@
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
-        <v>2.0833333333333332E-2</v>
+        <v>4.1666666666666666E-3</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>22</v>
@@ -1707,7 +1707,7 @@
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>2.4305555555555556E-2</v>
+        <v>4.8611111111111112E-3</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>24</v>
@@ -1777,7 +1777,7 @@
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
-        <v>2.7777777777777776E-2</v>
+        <v>5.5555555555555558E-3</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>40</v>
@@ -1849,7 +1849,7 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>3.125E-2</v>
+        <v>6.2499999999999995E-3</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>26</v>
@@ -1919,7 +1919,7 @@
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
-        <v>3.4722222222222224E-2</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>39</v>
@@ -1991,7 +1991,7 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
-        <v>3.8194444444444441E-2</v>
+        <v>7.6388888888888886E-3</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>41</v>
@@ -2061,7 +2061,7 @@
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333332E-3</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>43</v>
@@ -2133,7 +2133,7 @@
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
-        <v>4.5138888888888888E-2</v>
+        <v>9.0277777777777787E-3</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>42</v>
@@ -2203,7 +2203,7 @@
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>4.8611111111111112E-2</v>
+        <v>9.7222222222222224E-3</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>45</v>
@@ -2273,7 +2273,7 @@
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
-        <v>5.2083333333333336E-2</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>46</v>
@@ -2345,7 +2345,7 @@
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
-        <v>5.5555555555555552E-2</v>
+        <v>1.1111111111111112E-2</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>47</v>
@@ -2415,7 +2415,7 @@
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
-        <v>5.9027777777777783E-2</v>
+        <v>1.1805555555555555E-2</v>
       </c>
       <c r="B21" s="12" t="s">
         <v>56</v>
@@ -2485,7 +2485,7 @@
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
-        <v>6.25E-2</v>
+        <v>1.2499999999999999E-2</v>
       </c>
       <c r="B22" s="12" t="s">
         <v>31</v>
@@ -2557,7 +2557,7 @@
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>6.5972222222222224E-2</v>
+        <v>1.3194444444444444E-2</v>
       </c>
       <c r="B23" s="12" t="s">
         <v>44</v>
@@ -2627,7 +2627,7 @@
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
-        <v>6.9444444444444434E-2</v>
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>176</v>
@@ -2699,7 +2699,7 @@
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>7.2916666666666671E-2</v>
+        <v>1.4583333333333332E-2</v>
       </c>
       <c r="B25" s="12" t="s">
         <v>48</v>
@@ -2769,7 +2769,7 @@
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
-        <v>7.6388888888888895E-2</v>
+        <v>1.5277777777777777E-2</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>63</v>
@@ -2841,7 +2841,7 @@
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>7.9861111111111105E-2</v>
+        <v>1.5972222222222224E-2</v>
       </c>
       <c r="B27" s="12" t="s">
         <v>50</v>
@@ -2911,7 +2911,7 @@
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="11">
-        <v>8.3333333333333329E-2</v>
+        <v>1.6666666666666666E-2</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>49</v>
@@ -2983,7 +2983,7 @@
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>8.6805555555555566E-2</v>
+        <v>1.7361111111111112E-2</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>52</v>
@@ -3053,7 +3053,7 @@
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
-        <v>9.0277777777777776E-2</v>
+        <v>1.8055555555555557E-2</v>
       </c>
       <c r="B30" s="12" t="s">
         <v>53</v>
@@ -3123,7 +3123,7 @@
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>9.375E-2</v>
+        <v>1.8749999999999999E-2</v>
       </c>
       <c r="B31" s="12" t="s">
         <v>51</v>
@@ -3193,7 +3193,7 @@
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="11">
-        <v>9.7222222222222224E-2</v>
+        <v>1.9444444444444445E-2</v>
       </c>
       <c r="B32" s="12" t="s">
         <v>57</v>
@@ -3263,7 +3263,7 @@
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
-        <v>0.10069444444444443</v>
+        <v>2.013888888888889E-2</v>
       </c>
       <c r="B33" s="12" t="s">
         <v>44</v>
@@ -3333,7 +3333,7 @@
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" s="11">
-        <v>0.10416666666666667</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="B34" s="12" t="s">
         <v>54</v>
@@ -3403,7 +3403,7 @@
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" s="11">
-        <v>0.1076388888888889</v>
+        <v>2.1527777777777781E-2</v>
       </c>
       <c r="B35" s="12" t="s">
         <v>52</v>
@@ -3473,7 +3473,7 @@
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>0.1111111111111111</v>
+        <v>2.2222222222222223E-2</v>
       </c>
       <c r="B36" s="12" t="s">
         <v>52</v>
@@ -3543,7 +3543,7 @@
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" s="11">
-        <v>0.11458333333333333</v>
+        <v>2.2916666666666669E-2</v>
       </c>
       <c r="B37" s="12" t="s">
         <v>55</v>
@@ -3613,7 +3613,7 @@
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" s="11">
-        <v>0.11805555555555557</v>
+        <v>2.361111111111111E-2</v>
       </c>
       <c r="B38" s="12" t="s">
         <v>44</v>
@@ -3683,7 +3683,7 @@
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" s="11">
-        <v>0.12152777777777778</v>
+        <v>2.4305555555555556E-2</v>
       </c>
       <c r="B39" s="12" t="s">
         <v>39</v>
@@ -3753,7 +3753,7 @@
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" s="11">
-        <v>0.125</v>
+        <v>2.4999999999999998E-2</v>
       </c>
       <c r="B40" s="12" t="s">
         <v>66</v>
@@ -3823,7 +3823,7 @@
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>0.12847222222222224</v>
+        <v>2.5694444444444447E-2</v>
       </c>
       <c r="B41" s="12" t="s">
         <v>39</v>
@@ -3893,7 +3893,7 @@
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" s="11">
-        <v>0.13194444444444445</v>
+        <v>2.6388888888888889E-2</v>
       </c>
       <c r="B42" s="12" t="s">
         <v>44</v>
@@ -3963,7 +3963,7 @@
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>0.13541666666666666</v>
+        <v>2.7083333333333334E-2</v>
       </c>
       <c r="B43" s="12" t="s">
         <v>56</v>
@@ -4033,7 +4033,7 @@
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" s="11">
-        <v>0.1388888888888889</v>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="B44" s="12" t="s">
         <v>58</v>
@@ -4103,7 +4103,7 @@
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" s="11">
-        <v>0.1423611111111111</v>
+        <v>2.8472222222222222E-2</v>
       </c>
       <c r="B45" s="12" t="s">
         <v>59</v>
@@ -4173,7 +4173,7 @@
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46" s="11">
-        <v>0.14583333333333334</v>
+        <v>2.9166666666666664E-2</v>
       </c>
       <c r="B46" s="12" t="s">
         <v>44</v>
@@ -4243,7 +4243,7 @@
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" s="11">
-        <v>0.14930555555555555</v>
+        <v>2.9861111111111113E-2</v>
       </c>
       <c r="B47" s="12" t="s">
         <v>60</v>
@@ -4313,7 +4313,7 @@
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>0.15277777777777776</v>
+        <v>3.0555555555555555E-2</v>
       </c>
       <c r="B48" s="12" t="s">
         <v>61</v>

</xml_diff>

<commit_message>
Corrections in time vector
</commit_message>
<xml_diff>
--- a/DistributionSystems/SimulinkOpal/Device_Integration_Test_01/TestProcedure_detailed.xlsx
+++ b/DistributionSystems/SimulinkOpal/Device_Integration_Test_01/TestProcedure_detailed.xlsx
@@ -1026,8 +1026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1351,7 +1351,7 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
-        <v>2.3148148148148147E-5</v>
+        <v>3.4722222222222222E-5</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>44</v>

</xml_diff>